<commit_message>
Revising Annotation Guide for Interpretability feature
</commit_message>
<xml_diff>
--- a/responses/2039/Interp/T_interp_maybe.xlsx
+++ b/responses/2039/Interp/T_interp_maybe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
   <si>
     <t>the boy is playing with music</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>MD: agreed</t>
+  </si>
+  <si>
+    <t>annotators must make a judgement call about whether arguments are grammatically required. if "something" (or similar) fits as missing argument, OK (??)</t>
   </si>
 </sst>
 </file>
@@ -420,8 +423,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -441,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -449,6 +454,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -456,6 +462,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -787,9 +794,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R42" sqref="R42"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -914,7 +921,7 @@
         <v>81</v>
       </c>
       <c r="Q2" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:17">

</xml_diff>